<commit_message>
added query asked by customer as example
</commit_message>
<xml_diff>
--- a/src/it/resources/JSONPathTestBookIt.xlsx
+++ b/src/it/resources/JSONPathTestBookIt.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="74">
   <si>
     <t>Controllo</t>
   </si>
@@ -238,6 +238,12 @@
   </si>
   <si>
     <t>//a[@class=='pizzeria']</t>
+  </si>
+  <si>
+    <t>$.[?(@property === 'status' &amp;&amp; @ === '200')]</t>
+  </si>
+  <si>
+    <t>Verifica query PB 02 Versione Evoluta</t>
   </si>
 </sst>
 </file>
@@ -742,13 +748,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N29"/>
+  <dimension ref="A1:N30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="M6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="N13" sqref="N13"/>
+      <selection pane="bottomRight" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -894,120 +900,120 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>27</v>
+        <v>73</v>
       </c>
       <c r="M7" t="s">
         <v>17</v>
       </c>
       <c r="N7" t="s">
-        <v>20</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M8" t="s">
         <v>17</v>
       </c>
       <c r="N8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M9" t="s">
         <v>17</v>
       </c>
       <c r="N9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="M10" t="s">
         <v>17</v>
       </c>
       <c r="N10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M11" t="s">
         <v>17</v>
       </c>
       <c r="N11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="M12" s="19" t="s">
-        <v>2</v>
+        <v>31</v>
+      </c>
+      <c r="M12" t="s">
+        <v>17</v>
       </c>
       <c r="N12" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="M13" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="N13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="M13" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="N13" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>33</v>
       </c>
       <c r="M14" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="N14" s="2" t="s">
-        <v>64</v>
+      <c r="N14" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="M15" s="19" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="N15" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="M16" s="19" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="N16" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="M17" s="19" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="N17" s="2" t="s">
         <v>66</v>
@@ -1015,10 +1021,10 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M18" s="19" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="N18" s="2" t="s">
         <v>66</v>
@@ -1026,29 +1032,29 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="M19" s="19" t="s">
-        <v>43</v>
+        <v>41</v>
+      </c>
+      <c r="N19" s="2" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>44</v>
-      </c>
-      <c r="M20" t="s">
-        <v>45</v>
-      </c>
-      <c r="N20" s="2" t="s">
-        <v>67</v>
+        <v>42</v>
+      </c>
+      <c r="M20" s="19" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>46</v>
-      </c>
-      <c r="M21" s="19" t="s">
-        <v>47</v>
+        <v>44</v>
+      </c>
+      <c r="M21" t="s">
+        <v>45</v>
       </c>
       <c r="N21" s="2" t="s">
         <v>67</v>
@@ -1056,68 +1062,79 @@
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="M22" s="19" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="N22" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>50</v>
-      </c>
-      <c r="M23" s="20" t="s">
-        <v>57</v>
+        <v>48</v>
+      </c>
+      <c r="M23" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="N23" s="2" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M24" s="20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M25" s="20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="M26" s="20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M27" s="20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="M28" s="20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>55</v>
+      </c>
+      <c r="M29" s="20" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>56</v>
       </c>
-      <c r="M29" s="20" t="s">
+      <c r="M30" s="20" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1132,16 +1149,16 @@
     <mergeCell ref="M1:N1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="M14" r:id="rId1"/>
-    <hyperlink ref="M15" r:id="rId2"/>
-    <hyperlink ref="M16" r:id="rId3"/>
-    <hyperlink ref="M18" r:id="rId4"/>
-    <hyperlink ref="M17" r:id="rId5"/>
-    <hyperlink ref="M19" r:id="rId6"/>
-    <hyperlink ref="M21" r:id="rId7"/>
-    <hyperlink ref="M22" r:id="rId8"/>
-    <hyperlink ref="M12" r:id="rId9"/>
-    <hyperlink ref="M13" r:id="rId10"/>
+    <hyperlink ref="M15" r:id="rId1"/>
+    <hyperlink ref="M16" r:id="rId2"/>
+    <hyperlink ref="M17" r:id="rId3"/>
+    <hyperlink ref="M19" r:id="rId4"/>
+    <hyperlink ref="M18" r:id="rId5"/>
+    <hyperlink ref="M20" r:id="rId6"/>
+    <hyperlink ref="M22" r:id="rId7"/>
+    <hyperlink ref="M23" r:id="rId8"/>
+    <hyperlink ref="M13" r:id="rId9"/>
+    <hyperlink ref="M14" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId11"/>

</xml_diff>